<commit_message>
progress on data import script
</commit_message>
<xml_diff>
--- a/components/data/data.xlsx
+++ b/components/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron Goldstein\dev\VanBuilder\components\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8450A016-E194-4A58-A87D-D62161FC851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311D969-5F38-41A9-AFA2-87C830A884C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="704" activeTab="2" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="704" activeTab="1" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -56,27 +56,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>make </t>
-  </si>
-  <si>
-    <t>model </t>
-  </si>
-  <si>
-    <t>wheelbase </t>
-  </si>
-  <si>
-    <t>max_weight </t>
-  </si>
-  <si>
-    <t>engine </t>
-  </si>
-  <si>
-    <t>drive </t>
-  </si>
-  <si>
-    <t>passengers </t>
-  </si>
-  <si>
     <t>Framing</t>
   </si>
   <si>
@@ -173,9 +152,6 @@
     <t>Regular Unleaded V-6</t>
   </si>
   <si>
-    <t>Transmission</t>
-  </si>
-  <si>
     <t>Automatic</t>
   </si>
   <si>
@@ -191,12 +167,6 @@
     <t>Chassis Cab</t>
   </si>
   <si>
-    <t>external_width </t>
-  </si>
-  <si>
-    <t>external_height </t>
-  </si>
-  <si>
     <t>external_length</t>
   </si>
   <si>
@@ -218,9 +188,6 @@
     <t>cargo_length</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Water &amp; Plumbing</t>
   </si>
   <si>
@@ -282,6 +249,66 @@
   </si>
   <si>
     <t>ARKSEN 84"x 39"x 6" Universal Roof Rack Cargo Extension Car Top Luggage Holder Carrier Basket SUV Camping, Black</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>1" x 4"</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>1" x 1"</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>Aluminum framing material - price varies by length of component</t>
+  </si>
+  <si>
+    <t>Wood framing material - price varies by length of component</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>transmission</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>wheelbase</t>
+  </si>
+  <si>
+    <t>max_weight</t>
+  </si>
+  <si>
+    <t>engine</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>passengers</t>
+  </si>
+  <si>
+    <t>external_width</t>
+  </si>
+  <si>
+    <t>external_height</t>
   </si>
 </sst>
 </file>
@@ -334,13 +361,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -400,7 +428,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEFA8DCE-3388-4646-A460-38D7A2887001}" name="Table1" displayName="Table1" ref="A1:B14" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEFA8DCE-3388-4646-A460-38D7A2887001}" name="Categories" displayName="Categories" ref="A1:B14" totalsRowShown="0">
   <autoFilter ref="A1:B14" xr:uid="{CEFA8DCE-3388-4646-A460-38D7A2887001}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1C0A326E-6A63-4412-A0D4-0D12E73E5548}" name="name"/>
@@ -411,36 +439,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36555DEE-6402-4DAE-ACE1-2ED4CCCF61BD}" name="Table2" displayName="Table2" ref="A1:T8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36555DEE-6402-4DAE-ACE1-2ED4CCCF61BD}" name="Vans" displayName="Vans" ref="A1:T8" totalsRowShown="0">
   <autoFilter ref="A1:T8" xr:uid="{36555DEE-6402-4DAE-ACE1-2ED4CCCF61BD}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{4A2AA593-0576-4D95-92CF-03DAA474B385}" name="make "/>
-    <tableColumn id="2" xr3:uid="{432F6564-041E-4804-8638-42B7A821AC15}" name="model "/>
-    <tableColumn id="20" xr3:uid="{4D8805CA-AAC5-4C72-9325-6198CF739E4F}" name="Year"/>
-    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase " dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{4A2AA593-0576-4D95-92CF-03DAA474B385}" name="make"/>
+    <tableColumn id="2" xr3:uid="{432F6564-041E-4804-8638-42B7A821AC15}" name="model"/>
+    <tableColumn id="20" xr3:uid="{4D8805CA-AAC5-4C72-9325-6198CF739E4F}" name="year"/>
+    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase" dataDxfId="12"/>
     <tableColumn id="12" xr3:uid="{EA5EE0E9-A827-491E-9112-31EE08146CC3}" name="van_type"/>
-    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight " dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{83F69EBD-F948-4AED-B14D-0FCEAF1D3AB5}" name="engine "/>
-    <tableColumn id="13" xr3:uid="{802A4510-0C8F-46AB-B2E2-B9608C806A48}" name="Transmission"/>
-    <tableColumn id="8" xr3:uid="{67FFBE42-116B-4BFF-9420-BA0AA41CB4E5}" name="drive "/>
-    <tableColumn id="11" xr3:uid="{37371131-77CA-4603-A694-C8EC06648B35}" name="passengers "/>
-    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width " dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height " dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{83F69EBD-F948-4AED-B14D-0FCEAF1D3AB5}" name="engine"/>
+    <tableColumn id="13" xr3:uid="{802A4510-0C8F-46AB-B2E2-B9608C806A48}" name="transmission"/>
+    <tableColumn id="8" xr3:uid="{67FFBE42-116B-4BFF-9420-BA0AA41CB4E5}" name="drive"/>
+    <tableColumn id="11" xr3:uid="{37371131-77CA-4603-A694-C8EC06648B35}" name="passengers"/>
+    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}" name="Table3" displayName="Table3" ref="A1:K2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}" name="Exterior" displayName="Exterior" ref="A1:K2" totalsRowShown="0">
   <autoFilter ref="A1:K2" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0683B4BB-7F51-4927-9DA9-C1292867B7CD}" name="category "/>
@@ -454,6 +482,44 @@
     <tableColumn id="9" xr3:uid="{737EC8BB-3635-41DD-9F13-B6B134BAD492}" name="weight_per_unit "/>
     <tableColumn id="10" xr3:uid="{2E085D17-2A7F-4FFD-9783-C4A764C86A3A}" name="description "/>
     <tableColumn id="11" xr3:uid="{166AFEFE-C564-4CA9-8716-93FB001E7898}" name="other"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{043294C2-EEA3-4870-A9C2-411D02A66518}" name="Framing" displayName="Framing" ref="A1:J3" totalsRowShown="0">
+  <autoFilter ref="A1:J3" xr:uid="{043294C2-EEA3-4870-A9C2-411D02A66518}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{D1FB3D4D-F4EF-4287-BA5D-738CC147319F}" name="category "/>
+    <tableColumn id="2" xr3:uid="{64B55AB5-B8D6-47F9-B97E-A6FD601BFF96}" name="component"/>
+    <tableColumn id="3" xr3:uid="{0C7F0957-318F-4198-89C0-C2C08362D9CD}" name="item"/>
+    <tableColumn id="5" xr3:uid="{98187D51-4C84-4452-9C89-7FDF36F3BEB7}" name="material"/>
+    <tableColumn id="6" xr3:uid="{46F96AFB-14FB-4DE5-83BE-129B78D5298A}" name="dimensions"/>
+    <tableColumn id="7" xr3:uid="{DD77154B-5B22-4210-A2E7-BC9ED3C844F6}" name="unit_measure "/>
+    <tableColumn id="8" xr3:uid="{E040FE9C-12C2-462F-BFA9-8340259F3698}" name="cost_per_unit "/>
+    <tableColumn id="9" xr3:uid="{E8DE647C-5C1D-4CA5-8EA8-6832CA1E4A73}" name="weight_per_unit "/>
+    <tableColumn id="10" xr3:uid="{B71B3624-8ECF-4F82-BB34-68F027925C60}" name="description "/>
+    <tableColumn id="11" xr3:uid="{028628B3-09A5-427B-A231-893E22524F82}" name="other"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5A37213D-081D-4A9A-97FA-A6A049B75A73}" name="Insulation" displayName="Insulation" ref="A1:J2" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{5A37213D-081D-4A9A-97FA-A6A049B75A73}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{AC5A5AAC-5CF7-4E8C-B28E-89548F1F8EEC}" name="category "/>
+    <tableColumn id="2" xr3:uid="{DD83A9D3-2FFF-4487-8CE9-B3BCD503CA7A}" name="component"/>
+    <tableColumn id="3" xr3:uid="{28D97759-6277-4FD0-97ED-195C99902859}" name="item"/>
+    <tableColumn id="4" xr3:uid="{6B4C3B98-1E8E-47F6-8180-D8DF995B7AB9}" name="brand "/>
+    <tableColumn id="5" xr3:uid="{E4F18CB0-12FA-44F3-8FEA-F69C6895412E}" name="material"/>
+    <tableColumn id="6" xr3:uid="{B077278B-679B-4CEA-995F-52FB7D090F0C}" name="dimensions"/>
+    <tableColumn id="7" xr3:uid="{CE69B73D-E452-49CB-8BDD-8C0552A88B49}" name="unit_measure "/>
+    <tableColumn id="8" xr3:uid="{A2618B30-784C-4EB3-A433-BBF2DD6D2851}" name="cost_per_unit "/>
+    <tableColumn id="9" xr3:uid="{58BB0742-0945-4586-9229-66505B5269BC}" name="weight_per_unit "/>
+    <tableColumn id="10" xr3:uid="{B4540207-3471-41B9-BC0B-D05E0F6DE8B2}" name="description "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -760,7 +826,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,106 +845,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -972,8 +1038,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,72 +1062,72 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" t="s">
-        <v>54</v>
-      </c>
       <c r="Q1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="R1" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="S1" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="T1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>2021</v>
@@ -1070,7 +1136,7 @@
         <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2">
         <v>32285</v>
@@ -1080,13 +1146,13 @@
         <v>5234</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1095,15 +1161,9 @@
         <v>24</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
       <c r="R2" s="1">
         <v>80.7</v>
       </c>
@@ -1116,10 +1176,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>2021</v>
@@ -1128,7 +1188,7 @@
         <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2">
         <v>32935</v>
@@ -1138,13 +1198,13 @@
         <v>5173</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1153,15 +1213,9 @@
         <v>24</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1">
         <v>80.7</v>
       </c>
@@ -1174,10 +1228,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>2021</v>
@@ -1186,7 +1240,7 @@
         <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2">
         <v>34080</v>
@@ -1196,13 +1250,13 @@
         <v>3996</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1232,10 +1286,10 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>2021</v>
@@ -1244,7 +1298,7 @@
         <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2">
         <v>36135</v>
@@ -1254,13 +1308,13 @@
         <v>4005</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -1290,10 +1344,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>2021</v>
@@ -1302,7 +1356,7 @@
         <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2">
         <v>37885</v>
@@ -1312,13 +1366,13 @@
         <v>4427</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1348,10 +1402,10 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>2021</v>
@@ -1360,7 +1414,7 @@
         <v>159</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2">
         <v>39085</v>
@@ -1370,13 +1424,13 @@
         <v>3943</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1406,10 +1460,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>2021</v>
@@ -1418,7 +1472,7 @@
         <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F8" s="2">
         <v>42835</v>
@@ -1428,13 +1482,13 @@
         <v>4289</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1476,8 +1530,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,69 +1541,69 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>319.45999999999998</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1566,26 +1620,185 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A0846-AFF7-42F7-92F7-BF37DD01A404}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="4">
+        <f>18.51/6</f>
+        <v>3.0850000000000004</v>
+      </c>
+      <c r="H2">
+        <v>0.51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="4">
+        <f>5.17/8</f>
+        <v>0.64624999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D75A-618D-446B-8297-F21A108EB0E7}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1594,7 +1807,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" activeCellId="1" sqref="A1 H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
more progress on import module
</commit_message>
<xml_diff>
--- a/components/data/data.xlsx
+++ b/components/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron Goldstein\dev\VanBuilder\components\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311D969-5F38-41A9-AFA2-87C830A884C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D17385-B74B-47BF-BD9C-DBBD72781BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="704" activeTab="1" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="704" activeTab="4" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
   <si>
     <t>name</t>
   </si>
@@ -194,24 +194,6 @@
     <t>Flooring, Walls, &amp; Ceiling</t>
   </si>
   <si>
-    <t>category </t>
-  </si>
-  <si>
-    <t>brand </t>
-  </si>
-  <si>
-    <t>unit_measure </t>
-  </si>
-  <si>
-    <t>cost_per_unit </t>
-  </si>
-  <si>
-    <t>weight_per_unit </t>
-  </si>
-  <si>
-    <t>description </t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -309,6 +291,27 @@
   </si>
   <si>
     <t>external_height</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>unit_measure</t>
+  </si>
+  <si>
+    <t>cost_per_unit</t>
+  </si>
+  <si>
+    <t>weight_per_unit</t>
+  </si>
+  <si>
+    <t>Reflectix</t>
+  </si>
+  <si>
+    <t>HeatInsulation</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,20 +342,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -361,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -369,12 +406,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -445,23 +491,23 @@
     <tableColumn id="1" xr3:uid="{4A2AA593-0576-4D95-92CF-03DAA474B385}" name="make"/>
     <tableColumn id="2" xr3:uid="{432F6564-041E-4804-8638-42B7A821AC15}" name="model"/>
     <tableColumn id="20" xr3:uid="{4D8805CA-AAC5-4C72-9325-6198CF739E4F}" name="year"/>
-    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase" dataDxfId="14"/>
     <tableColumn id="12" xr3:uid="{EA5EE0E9-A827-491E-9112-31EE08146CC3}" name="van_type"/>
-    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="11" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{83F69EBD-F948-4AED-B14D-0FCEAF1D3AB5}" name="engine"/>
     <tableColumn id="13" xr3:uid="{802A4510-0C8F-46AB-B2E2-B9608C806A48}" name="transmission"/>
     <tableColumn id="8" xr3:uid="{67FFBE42-116B-4BFF-9420-BA0AA41CB4E5}" name="drive"/>
     <tableColumn id="11" xr3:uid="{37371131-77CA-4603-A694-C8EC06648B35}" name="passengers"/>
-    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -471,16 +517,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}" name="Exterior" displayName="Exterior" ref="A1:K2" totalsRowShown="0">
   <autoFilter ref="A1:K2" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0683B4BB-7F51-4927-9DA9-C1292867B7CD}" name="category "/>
+    <tableColumn id="1" xr3:uid="{0683B4BB-7F51-4927-9DA9-C1292867B7CD}" name="category"/>
     <tableColumn id="2" xr3:uid="{BF15DA8F-8A03-4BE8-ADE7-64FAF4CE8F2B}" name="component"/>
     <tableColumn id="3" xr3:uid="{237AEE53-F308-4344-9D15-659F88572AA3}" name="item"/>
-    <tableColumn id="4" xr3:uid="{22A1BAD4-83B8-4CCB-8FD5-BAB35E36CCAC}" name="brand "/>
-    <tableColumn id="5" xr3:uid="{269B84AB-42EC-40AA-8684-853C887541D8}" name="material" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{22A1BAD4-83B8-4CCB-8FD5-BAB35E36CCAC}" name="brand"/>
+    <tableColumn id="5" xr3:uid="{269B84AB-42EC-40AA-8684-853C887541D8}" name="material" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{04979A69-F9E3-4E7B-A98F-28F1D05B1733}" name="dimensions"/>
-    <tableColumn id="7" xr3:uid="{DD894E4F-E914-44F6-9FDF-A696F40CC59F}" name="unit_measure "/>
-    <tableColumn id="8" xr3:uid="{3170A307-E030-456A-AD00-1C8135CF363D}" name="cost_per_unit "/>
-    <tableColumn id="9" xr3:uid="{737EC8BB-3635-41DD-9F13-B6B134BAD492}" name="weight_per_unit "/>
-    <tableColumn id="10" xr3:uid="{2E085D17-2A7F-4FFD-9783-C4A764C86A3A}" name="description "/>
+    <tableColumn id="7" xr3:uid="{DD894E4F-E914-44F6-9FDF-A696F40CC59F}" name="unit_measure"/>
+    <tableColumn id="8" xr3:uid="{3170A307-E030-456A-AD00-1C8135CF363D}" name="cost_per_unit"/>
+    <tableColumn id="9" xr3:uid="{737EC8BB-3635-41DD-9F13-B6B134BAD492}" name="weight_per_unit"/>
+    <tableColumn id="10" xr3:uid="{2E085D17-2A7F-4FFD-9783-C4A764C86A3A}" name="description"/>
     <tableColumn id="11" xr3:uid="{166AFEFE-C564-4CA9-8716-93FB001E7898}" name="other"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -491,35 +537,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{043294C2-EEA3-4870-A9C2-411D02A66518}" name="Framing" displayName="Framing" ref="A1:J3" totalsRowShown="0">
   <autoFilter ref="A1:J3" xr:uid="{043294C2-EEA3-4870-A9C2-411D02A66518}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D1FB3D4D-F4EF-4287-BA5D-738CC147319F}" name="category "/>
-    <tableColumn id="2" xr3:uid="{64B55AB5-B8D6-47F9-B97E-A6FD601BFF96}" name="component"/>
-    <tableColumn id="3" xr3:uid="{0C7F0957-318F-4198-89C0-C2C08362D9CD}" name="item"/>
+    <tableColumn id="1" xr3:uid="{D1FB3D4D-F4EF-4287-BA5D-738CC147319F}" name="category"/>
+    <tableColumn id="2" xr3:uid="{64B55AB5-B8D6-47F9-B97E-A6FD601BFF96}" name="component" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0C7F0957-318F-4198-89C0-C2C08362D9CD}" name="item" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{98187D51-4C84-4452-9C89-7FDF36F3BEB7}" name="material"/>
     <tableColumn id="6" xr3:uid="{46F96AFB-14FB-4DE5-83BE-129B78D5298A}" name="dimensions"/>
-    <tableColumn id="7" xr3:uid="{DD77154B-5B22-4210-A2E7-BC9ED3C844F6}" name="unit_measure "/>
-    <tableColumn id="8" xr3:uid="{E040FE9C-12C2-462F-BFA9-8340259F3698}" name="cost_per_unit "/>
-    <tableColumn id="9" xr3:uid="{E8DE647C-5C1D-4CA5-8EA8-6832CA1E4A73}" name="weight_per_unit "/>
-    <tableColumn id="10" xr3:uid="{B71B3624-8ECF-4F82-BB34-68F027925C60}" name="description "/>
+    <tableColumn id="7" xr3:uid="{DD77154B-5B22-4210-A2E7-BC9ED3C844F6}" name="unit_measure"/>
+    <tableColumn id="8" xr3:uid="{E040FE9C-12C2-462F-BFA9-8340259F3698}" name="cost_per_unit"/>
+    <tableColumn id="9" xr3:uid="{E8DE647C-5C1D-4CA5-8EA8-6832CA1E4A73}" name="weight_per_unit"/>
+    <tableColumn id="10" xr3:uid="{B71B3624-8ECF-4F82-BB34-68F027925C60}" name="description"/>
     <tableColumn id="11" xr3:uid="{028628B3-09A5-427B-A231-893E22524F82}" name="other"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5A37213D-081D-4A9A-97FA-A6A049B75A73}" name="Insulation" displayName="Insulation" ref="A1:J2" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{5A37213D-081D-4A9A-97FA-A6A049B75A73}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{AC5A5AAC-5CF7-4E8C-B28E-89548F1F8EEC}" name="category "/>
-    <tableColumn id="2" xr3:uid="{DD83A9D3-2FFF-4487-8CE9-B3BCD503CA7A}" name="component"/>
-    <tableColumn id="3" xr3:uid="{28D97759-6277-4FD0-97ED-195C99902859}" name="item"/>
-    <tableColumn id="4" xr3:uid="{6B4C3B98-1E8E-47F6-8180-D8DF995B7AB9}" name="brand "/>
-    <tableColumn id="5" xr3:uid="{E4F18CB0-12FA-44F3-8FEA-F69C6895412E}" name="material"/>
-    <tableColumn id="6" xr3:uid="{B077278B-679B-4CEA-995F-52FB7D090F0C}" name="dimensions"/>
-    <tableColumn id="7" xr3:uid="{CE69B73D-E452-49CB-8BDD-8C0552A88B49}" name="unit_measure "/>
-    <tableColumn id="8" xr3:uid="{A2618B30-784C-4EB3-A433-BBF2DD6D2851}" name="cost_per_unit "/>
-    <tableColumn id="9" xr3:uid="{58BB0742-0945-4586-9229-66505B5269BC}" name="weight_per_unit "/>
-    <tableColumn id="10" xr3:uid="{B4540207-3471-41B9-BC0B-D05E0F6DE8B2}" name="description "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -826,16 +853,16 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="139.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,15 +870,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -859,7 +886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -867,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -875,7 +902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -883,7 +910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -891,7 +918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -899,7 +926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -907,7 +934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -915,7 +942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -923,7 +950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -931,7 +958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -939,7 +966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -962,7 +989,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -975,7 +1002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -988,7 +1015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1001,7 +1028,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1014,7 +1041,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1027,7 +1054,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1038,40 +1065,40 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:Q3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="17" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.41796875" customWidth="1"/>
+    <col min="2" max="3" width="20.83984375" customWidth="1"/>
+    <col min="4" max="5" width="13.26171875" customWidth="1"/>
+    <col min="6" max="6" width="12.26171875" customWidth="1"/>
+    <col min="7" max="7" width="12.83984375" customWidth="1"/>
+    <col min="8" max="8" width="14.41796875" customWidth="1"/>
+    <col min="9" max="9" width="20.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.41796875" customWidth="1"/>
+    <col min="11" max="11" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.41796875" customWidth="1"/>
+    <col min="13" max="17" width="12.26171875" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.26171875" customWidth="1"/>
+    <col min="20" max="20" width="9.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -1083,19 +1110,19 @@
         <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
-        <v>83</v>
-      </c>
       <c r="L1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s">
         <v>35</v>
@@ -1113,16 +1140,16 @@
         <v>45</v>
       </c>
       <c r="R1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="S1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="T1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1174,7 +1201,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1253,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1284,7 +1311,7 @@
         <v>195.4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1342,7 +1369,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1400,7 +1427,7 @@
         <v>250.6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1458,7 +1485,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1531,67 +1558,67 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="12" width="18.42578125" customWidth="1"/>
+    <col min="1" max="12" width="18.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>42</v>
@@ -1600,13 +1627,13 @@
         <v>319.45999999999998</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E5" s="3"/>
     </row>
   </sheetData>
@@ -1623,71 +1650,71 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.15625" customWidth="1"/>
+    <col min="2" max="2" width="13.26171875" customWidth="1"/>
+    <col min="4" max="4" width="10.578125" customWidth="1"/>
+    <col min="5" max="5" width="13.41796875" customWidth="1"/>
+    <col min="6" max="6" width="15.83984375" customWidth="1"/>
+    <col min="7" max="7" width="15.68359375" customWidth="1"/>
+    <col min="8" max="8" width="18.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G2" s="4">
         <f>18.51/6</f>
@@ -1697,27 +1724,27 @@
         <v>0.51</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
       </c>
       <c r="G3" s="4">
         <f>5.17/8</f>
@@ -1727,7 +1754,7 @@
         <v>1.3</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1741,64 +1768,79 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D75A-618D-446B-8297-F21A108EB0E7}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.15625" customWidth="1"/>
+    <col min="2" max="2" width="13.26171875" customWidth="1"/>
+    <col min="5" max="5" width="10.578125" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" customWidth="1"/>
+    <col min="7" max="7" width="15.83984375" customWidth="1"/>
+    <col min="8" max="8" width="15.68359375" customWidth="1"/>
+    <col min="9" max="9" width="18.26171875" customWidth="1"/>
+    <col min="10" max="10" width="13.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -1811,7 +1853,7 @@
       <selection activeCell="H6" activeCellId="1" sqref="A1 H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1824,7 +1866,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1837,7 +1879,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1852,7 +1894,7 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working on api views
</commit_message>
<xml_diff>
--- a/components/data/data.xlsx
+++ b/components/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron Goldstein\dev\VanBuilder\components\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D17385-B74B-47BF-BD9C-DBBD72781BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF40C6AD-6555-4A07-9FD6-BA7C3CFF1CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="704" activeTab="4" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="704" activeTab="2" xr2:uid="{A38B9A29-454D-4096-BDD3-E3B191CFC3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>name</t>
   </si>
@@ -215,19 +215,10 @@
     <t>Roof Rack</t>
   </si>
   <si>
-    <t>RoofRack</t>
-  </si>
-  <si>
     <t>ARKSEN</t>
   </si>
   <si>
     <t xml:space="preserve">84"x 39"x 6" </t>
-  </si>
-  <si>
-    <t>46.3 pounds</t>
-  </si>
-  <si>
-    <t>Alloy Steel, Metal</t>
   </si>
   <si>
     <t>ARKSEN 84"x 39"x 6" Universal Roof Rack Cargo Extension Car Top Luggage Holder Carrier Basket SUV Camping, Black</t>
@@ -398,13 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -414,15 +402,12 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="14">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -491,43 +476,40 @@
     <tableColumn id="1" xr3:uid="{4A2AA593-0576-4D95-92CF-03DAA474B385}" name="make"/>
     <tableColumn id="2" xr3:uid="{432F6564-041E-4804-8638-42B7A821AC15}" name="model"/>
     <tableColumn id="20" xr3:uid="{4D8805CA-AAC5-4C72-9325-6198CF739E4F}" name="year"/>
-    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{86E4C40F-F28F-4ED4-88E3-F0EF119969DD}" name="wheelbase" dataDxfId="13"/>
     <tableColumn id="12" xr3:uid="{EA5EE0E9-A827-491E-9112-31EE08146CC3}" name="van_type"/>
-    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="13" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{A24E6374-ED0E-4CD4-9D0C-8CEB485182E4}" name="price_new" dataDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{80820585-58F3-493A-AC56-E83DC56778F9}" name="price_used" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F1004D73-DF0F-4E95-BF89-74D527194FF8}" name="max_weight" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{83F69EBD-F948-4AED-B14D-0FCEAF1D3AB5}" name="engine"/>
     <tableColumn id="13" xr3:uid="{802A4510-0C8F-46AB-B2E2-B9608C806A48}" name="transmission"/>
     <tableColumn id="8" xr3:uid="{67FFBE42-116B-4BFF-9420-BA0AA41CB4E5}" name="drive"/>
     <tableColumn id="11" xr3:uid="{37371131-77CA-4603-A694-C8EC06648B35}" name="passengers"/>
-    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{FB801262-A003-4858-9558-A1DABCE64DA4}" name="fuel_tank" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{3A96C0E2-3CA0-4CD6-8537-9962ED66AFB3}" name="mpg" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{B38FDFB6-27E7-4B8A-9140-C9B0B7B96B3C}" name="cargo_width" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{F8302EE3-6C9C-440B-9137-5094BC22959F}" name="cargo_height" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{75A79DC1-00C3-4D90-A005-E601118E1352}" name="cargo_length" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{B070AD98-3433-44C0-9D39-4BAD019EDEB9}" name="external_width" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{9C992F68-9133-47E1-AC13-D84FBB6D812B}" name="external_height" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{43010E41-3D71-4FA8-9EFD-5C3A7C51473A}" name="external_length" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}" name="Exterior" displayName="Exterior" ref="A1:K2" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}" name="Exterior" displayName="Exterior" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{7746306F-8EB2-4041-B00B-1A2D93A6733E}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0683B4BB-7F51-4927-9DA9-C1292867B7CD}" name="category"/>
-    <tableColumn id="2" xr3:uid="{BF15DA8F-8A03-4BE8-ADE7-64FAF4CE8F2B}" name="component"/>
-    <tableColumn id="3" xr3:uid="{237AEE53-F308-4344-9D15-659F88572AA3}" name="item"/>
+    <tableColumn id="3" xr3:uid="{237AEE53-F308-4344-9D15-659F88572AA3}" name="component"/>
     <tableColumn id="4" xr3:uid="{22A1BAD4-83B8-4CCB-8FD5-BAB35E36CCAC}" name="brand"/>
-    <tableColumn id="5" xr3:uid="{269B84AB-42EC-40AA-8684-853C887541D8}" name="material" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{04979A69-F9E3-4E7B-A98F-28F1D05B1733}" name="dimensions"/>
     <tableColumn id="7" xr3:uid="{DD894E4F-E914-44F6-9FDF-A696F40CC59F}" name="unit_measure"/>
     <tableColumn id="8" xr3:uid="{3170A307-E030-456A-AD00-1C8135CF363D}" name="cost_per_unit"/>
     <tableColumn id="9" xr3:uid="{737EC8BB-3635-41DD-9F13-B6B134BAD492}" name="weight_per_unit"/>
     <tableColumn id="10" xr3:uid="{2E085D17-2A7F-4FFD-9783-C4A764C86A3A}" name="description"/>
-    <tableColumn id="11" xr3:uid="{166AFEFE-C564-4CA9-8716-93FB001E7898}" name="other"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -856,13 +838,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="139.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -878,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -886,7 +868,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -894,7 +876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -902,7 +884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -910,7 +892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -918,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -926,7 +908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -934,7 +916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -942,7 +924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -950,7 +932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -958,7 +940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -966,7 +948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -989,7 +971,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1002,7 +984,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1015,7 +997,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1028,7 +1010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1041,7 +1023,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1054,7 +1036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1069,36 +1051,36 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.41796875" customWidth="1"/>
-    <col min="2" max="3" width="20.83984375" customWidth="1"/>
-    <col min="4" max="5" width="13.26171875" customWidth="1"/>
-    <col min="6" max="6" width="12.26171875" customWidth="1"/>
-    <col min="7" max="7" width="12.83984375" customWidth="1"/>
-    <col min="8" max="8" width="14.41796875" customWidth="1"/>
-    <col min="9" max="9" width="20.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.41796875" customWidth="1"/>
-    <col min="11" max="11" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.41796875" customWidth="1"/>
-    <col min="13" max="17" width="12.26171875" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="17" width="12.28515625" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="12.26171875" customWidth="1"/>
-    <col min="20" max="20" width="9.26171875" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -1110,19 +1092,19 @@
         <v>41</v>
       </c>
       <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
       </c>
       <c r="M1" t="s">
         <v>35</v>
@@ -1140,16 +1122,16 @@
         <v>45</v>
       </c>
       <c r="R1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="S1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="T1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1201,7 +1183,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1253,7 +1235,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1293,7 @@
         <v>195.4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1351,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1427,7 +1409,7 @@
         <v>250.6</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1485,7 +1467,7 @@
         <v>232.6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1555,86 +1537,68 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D9ACB2-091C-4B60-B61F-14F16F5233E3}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="18.41796875" customWidth="1"/>
+    <col min="1" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
         <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
       <c r="H1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>319.45999999999998</v>
+      </c>
+      <c r="G2">
+        <v>46.3</v>
+      </c>
+      <c r="H2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2">
-        <v>319.45999999999998</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1653,21 +1617,21 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.15625" customWidth="1"/>
-    <col min="2" max="2" width="13.26171875" customWidth="1"/>
-    <col min="4" max="4" width="10.578125" customWidth="1"/>
-    <col min="5" max="5" width="13.41796875" customWidth="1"/>
-    <col min="6" max="6" width="15.83984375" customWidth="1"/>
-    <col min="7" max="7" width="15.68359375" customWidth="1"/>
-    <col min="8" max="8" width="18.26171875" customWidth="1"/>
-    <col min="9" max="9" width="13.578125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
         <v>52</v>
@@ -1682,13 +1646,13 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -1697,26 +1661,26 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>65</v>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
       <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="4">
+        <v>64</v>
+      </c>
+      <c r="G2" s="3">
         <f>18.51/6</f>
         <v>3.0850000000000004</v>
       </c>
@@ -1724,29 +1688,29 @@
         <v>0.51</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f>5.17/8</f>
         <v>0.64624999999999999</v>
       </c>
@@ -1754,7 +1718,7 @@
         <v>1.3</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1768,76 +1732,73 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36D75A-618D-446B-8297-F21A108EB0E7}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.15625" customWidth="1"/>
-    <col min="2" max="2" width="13.26171875" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="6" max="6" width="13.41796875" customWidth="1"/>
-    <col min="7" max="7" width="15.83984375" customWidth="1"/>
-    <col min="8" max="8" width="15.68359375" customWidth="1"/>
-    <col min="9" max="9" width="18.26171875" customWidth="1"/>
-    <col min="10" max="10" width="13.578125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1853,7 +1814,7 @@
       <selection activeCell="H6" activeCellId="1" sqref="A1 H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1866,7 +1827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1879,7 +1840,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1894,7 +1855,7 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>